<commit_message>
Update 03 from swiseWHAT account
</commit_message>
<xml_diff>
--- a/Submission-01/IP01 - Calculator Test Cases.xlsx
+++ b/Submission-01/IP01 - Calculator Test Cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Saman\Desktop\CS 504\4. Individual Project\CS504-Individual-Project-Hipples\Submission-01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swiseWHAT\Desktop\CS504-Individual-Project-Hipples\Submission-01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6008F11-D3C6-4863-A952-12E62934C168}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1757530-34F5-4130-83BE-26641ADA2105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{7A704EFB-4689-47B1-91E6-B7D4900305AC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>what</t>
   </si>
@@ -351,31 +351,17 @@
     <t>tc_github_03</t>
   </si>
   <si>
+    <t>github check-in, attempt 2</t>
+  </si>
+  <si>
+    <t>x. able to pass tc_github_01
+x. creation of swiseWHAT Window's account completed</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">1. sign in to swiseWHAT's windows account and repeat tc_github_01
-2. open cmd prompt
-3. set directory to the newly cloned repository
-4. type the three following commands into cmd: 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t>1. sign in to swiseWHAT's windows account and repeat tc_github_01 to create newly cloned hipples repository
+2. open, edit, then save this test case document
+3. open cmd prompt and set directory to the newly cloned repository, push "Update 03 from swiseWHAT account"</t>
     </r>
     <r>
       <rPr>
@@ -385,58 +371,7 @@
         <rFont val="Palatino Linotype"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">git add .
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t>2.</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> git commit -m "Update 02 from swiseWHAT account"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">3. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Palatino Linotype"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">git push origin main
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -889,6 +824,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -930,18 +877,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1313,6 +1248,121 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>156952</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91441</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1353292</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>33243</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEA13407-8204-4F02-8A61-AE473F94C2C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3739342" y="5742116"/>
+          <a:ext cx="8321534" cy="6681049"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>65388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>143308</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0B14932-ADA0-4A77-953A-5073474FAC47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="5923882"/>
+          <a:ext cx="3673830" cy="1859218"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1686,699 +1736,699 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="41"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="41"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="41"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="41"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="41"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="41"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="41"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="41"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="41"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="41"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="41"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="37"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="37"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="41"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="37"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="41"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="37"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="41"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="37"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="41"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="37"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="41"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="37"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="41"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="37"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="41"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="41"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="37"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="37"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="41"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="41"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="41"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="39"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="35"/>
     </row>
     <row r="65" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="32"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
-      <c r="I65" s="33"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="36"/>
+      <c r="G65" s="36"/>
+      <c r="H65" s="36"/>
+      <c r="I65" s="37"/>
     </row>
     <row r="66" spans="1:9" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A66" s="10"/>
@@ -2422,7 +2472,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="30" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -2452,728 +2502,728 @@
       <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" s="19" customFormat="1" ht="312" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="E2" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="43" t="s">
+      <c r="I2" s="29" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="41"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="41"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="41"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="41"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="41"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="41"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="41"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="41"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="41"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="41"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="41"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="37"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="37"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="41"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="37"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="41"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="37"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="41"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="37"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="41"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="37"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="41"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="37"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="41"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="37"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="41"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="41"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="37"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="37"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="41"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="41"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="41"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="39"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="35"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="40"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="41"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="45"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="26"/>
@@ -4918,8 +4968,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59EC7F2-2576-421B-9507-AC581ABE249C}">
   <dimension ref="A1:K198"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="77" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4933,7 +4983,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="21" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="30" t="s">
         <v>49</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -4962,729 +5012,721 @@
       </c>
       <c r="J1" s="20"/>
     </row>
-    <row r="2" spans="1:10" s="19" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:10" s="19" customFormat="1" ht="409.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="42" t="s">
+      <c r="B2" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="C2" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="43" t="s">
-        <v>67</v>
-      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="29"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="35"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="37"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="36"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="36"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="37"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="36"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="37"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="36"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="36"/>
-      <c r="I11" s="37"/>
+      <c r="A11" s="40"/>
+      <c r="B11" s="40"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="36"/>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="37"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="41"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="36"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="37"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="36"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="41"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="36"/>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="37"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="37"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="36"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="36"/>
-      <c r="I17" s="37"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="41"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="36"/>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="41"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="41"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="36"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="36"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="41"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="37"/>
+      <c r="A21" s="40"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="36"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="37"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="36"/>
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="37"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="41"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="36"/>
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="37"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="41"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="36"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="37"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="40"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="41"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="36"/>
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="37"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40"/>
+      <c r="E26" s="40"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="40"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="41"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="36"/>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="37"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="40"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="41"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="37"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="41"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="36"/>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="37"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="41"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="36"/>
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="37"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="41"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="36"/>
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="37"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="41"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="36"/>
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="37"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="41"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="37"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="41"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="36"/>
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="37"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="41"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="37"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
+      <c r="C35" s="40"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="40"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="41"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="37"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="41"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="37"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="40"/>
+      <c r="G37" s="40"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="41"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="37"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="41"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="37"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="40"/>
+      <c r="H39" s="40"/>
+      <c r="I39" s="41"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
+      <c r="A40" s="40"/>
+      <c r="B40" s="40"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="40"/>
+      <c r="H40" s="40"/>
+      <c r="I40" s="41"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="37"/>
+      <c r="A41" s="40"/>
+      <c r="B41" s="40"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="40"/>
+      <c r="I41" s="41"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="37"/>
+      <c r="A42" s="40"/>
+      <c r="B42" s="40"/>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="40"/>
+      <c r="I42" s="41"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="37"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="41"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="37"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="40"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="41"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="37"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="41"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="37"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="40"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="40"/>
+      <c r="I46" s="41"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="36"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
+      <c r="A47" s="40"/>
+      <c r="B47" s="40"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="40"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="40"/>
+      <c r="I47" s="41"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="36"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="37"/>
+      <c r="A48" s="40"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="41"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="36"/>
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="37"/>
+      <c r="A49" s="40"/>
+      <c r="B49" s="40"/>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="40"/>
+      <c r="G49" s="40"/>
+      <c r="H49" s="40"/>
+      <c r="I49" s="41"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="36"/>
-      <c r="B50" s="36"/>
-      <c r="C50" s="36"/>
-      <c r="D50" s="36"/>
-      <c r="E50" s="36"/>
-      <c r="F50" s="36"/>
-      <c r="G50" s="36"/>
-      <c r="H50" s="36"/>
-      <c r="I50" s="37"/>
+      <c r="A50" s="40"/>
+      <c r="B50" s="40"/>
+      <c r="C50" s="40"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="40"/>
+      <c r="G50" s="40"/>
+      <c r="H50" s="40"/>
+      <c r="I50" s="41"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="36"/>
-      <c r="B51" s="36"/>
-      <c r="C51" s="36"/>
-      <c r="D51" s="36"/>
-      <c r="E51" s="36"/>
-      <c r="F51" s="36"/>
-      <c r="G51" s="36"/>
-      <c r="H51" s="36"/>
-      <c r="I51" s="37"/>
+      <c r="A51" s="40"/>
+      <c r="B51" s="40"/>
+      <c r="C51" s="40"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="40"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="40"/>
+      <c r="I51" s="41"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="36"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="36"/>
-      <c r="D52" s="36"/>
-      <c r="E52" s="36"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="36"/>
-      <c r="H52" s="36"/>
-      <c r="I52" s="37"/>
+      <c r="A52" s="40"/>
+      <c r="B52" s="40"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="40"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="40"/>
+      <c r="I52" s="41"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="36"/>
-      <c r="B53" s="36"/>
-      <c r="C53" s="36"/>
-      <c r="D53" s="36"/>
-      <c r="E53" s="36"/>
-      <c r="F53" s="36"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="37"/>
+      <c r="A53" s="40"/>
+      <c r="B53" s="40"/>
+      <c r="C53" s="40"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="40"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="40"/>
+      <c r="I53" s="41"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="36"/>
-      <c r="B54" s="36"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="36"/>
-      <c r="F54" s="36"/>
-      <c r="G54" s="36"/>
-      <c r="H54" s="36"/>
-      <c r="I54" s="37"/>
+      <c r="A54" s="40"/>
+      <c r="B54" s="40"/>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="40"/>
+      <c r="G54" s="40"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="41"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="36"/>
-      <c r="B55" s="36"/>
-      <c r="C55" s="36"/>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="37"/>
+      <c r="A55" s="40"/>
+      <c r="B55" s="40"/>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="40"/>
+      <c r="G55" s="40"/>
+      <c r="H55" s="40"/>
+      <c r="I55" s="41"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="36"/>
-      <c r="B56" s="36"/>
-      <c r="C56" s="36"/>
-      <c r="D56" s="36"/>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="37"/>
+      <c r="A56" s="40"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="41"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="36"/>
-      <c r="B57" s="36"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="36"/>
-      <c r="G57" s="36"/>
-      <c r="H57" s="36"/>
-      <c r="I57" s="37"/>
+      <c r="A57" s="40"/>
+      <c r="B57" s="40"/>
+      <c r="C57" s="40"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="40"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="40"/>
+      <c r="I57" s="41"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="36"/>
-      <c r="B58" s="36"/>
-      <c r="C58" s="36"/>
-      <c r="D58" s="36"/>
-      <c r="E58" s="36"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="36"/>
-      <c r="H58" s="36"/>
-      <c r="I58" s="37"/>
+      <c r="A58" s="40"/>
+      <c r="B58" s="40"/>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="40"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="40"/>
+      <c r="I58" s="41"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="36"/>
-      <c r="B59" s="36"/>
-      <c r="C59" s="36"/>
-      <c r="D59" s="36"/>
-      <c r="E59" s="36"/>
-      <c r="F59" s="36"/>
-      <c r="G59" s="36"/>
-      <c r="H59" s="36"/>
-      <c r="I59" s="37"/>
+      <c r="A59" s="40"/>
+      <c r="B59" s="40"/>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="40"/>
+      <c r="G59" s="40"/>
+      <c r="H59" s="40"/>
+      <c r="I59" s="41"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="36"/>
-      <c r="B60" s="36"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="36"/>
-      <c r="F60" s="36"/>
-      <c r="G60" s="36"/>
-      <c r="H60" s="36"/>
-      <c r="I60" s="37"/>
+      <c r="A60" s="40"/>
+      <c r="B60" s="40"/>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
+      <c r="F60" s="40"/>
+      <c r="G60" s="40"/>
+      <c r="H60" s="40"/>
+      <c r="I60" s="41"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="36"/>
-      <c r="B61" s="36"/>
-      <c r="C61" s="36"/>
-      <c r="D61" s="36"/>
-      <c r="E61" s="36"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="36"/>
-      <c r="H61" s="36"/>
-      <c r="I61" s="37"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="40"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+      <c r="I61" s="41"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="36"/>
-      <c r="B62" s="36"/>
-      <c r="C62" s="36"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="36"/>
-      <c r="G62" s="36"/>
-      <c r="H62" s="36"/>
-      <c r="I62" s="37"/>
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+      <c r="I62" s="41"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="38"/>
-      <c r="B63" s="38"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="38"/>
-      <c r="E63" s="38"/>
-      <c r="F63" s="38"/>
-      <c r="G63" s="38"/>
-      <c r="H63" s="38"/>
-      <c r="I63" s="39"/>
+      <c r="A63" s="42"/>
+      <c r="B63" s="42"/>
+      <c r="C63" s="42"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="42"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="42"/>
+      <c r="H63" s="42"/>
+      <c r="I63" s="43"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
+      <c r="A64" s="34"/>
+      <c r="B64" s="34"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="34"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="35"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="40"/>
-      <c r="B65" s="40"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="40"/>
-      <c r="F65" s="40"/>
-      <c r="G65" s="40"/>
-      <c r="H65" s="40"/>
-      <c r="I65" s="41"/>
+      <c r="A65" s="44"/>
+      <c r="B65" s="44"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
+      <c r="F65" s="44"/>
+      <c r="G65" s="44"/>
+      <c r="H65" s="44"/>
+      <c r="I65" s="45"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A66" s="26"/>
@@ -7420,6 +7462,7 @@
     <mergeCell ref="A64:I65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>